<commit_message>
Tests technologiques + fiches techniques
</commit_message>
<xml_diff>
--- a/Analyse/fiches techniques produits existants.xlsx
+++ b/Analyse/fiches techniques produits existants.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr checkCompatibility="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gregory/Desktop/hes-so/3 eme/Projet de semestre/PS2/SAS/Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\3eme annee\SAS\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="460" windowWidth="28800" windowHeight="19600" tabRatio="500"/>
+    <workbookView xWindow="5940" yWindow="465" windowWidth="28800" windowHeight="19605" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Blocage</t>
   </si>
@@ -150,6 +147,98 @@
   </si>
   <si>
     <t xml:space="preserve">Ce logiciel est très solide et permet de bien gérer d'un point de vue administrateur. Mais il ne permet pas à l'utilisateur de prendre conscience du temps qu'il passe sur telle ou telle application. L'idéal serait qu'il sorte des statistiques d'utilisations </t>
+  </si>
+  <si>
+    <t>Contrôle parental Swisscom</t>
+  </si>
+  <si>
+    <t>Fonctionne pour tout ordinateur, tablette et smartphone pouvant se connecter à internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne fonctionne que sur la base de restrictions. L'utilisateur du réseau contrôlé ne peut pas changer quoi que ce soit aux restrictions, il subit des interdits. </t>
+  </si>
+  <si>
+    <t>Les enfants particulièrement
+et les adolescents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne donne aucun contrôle. L'application
+interdit mais n'apprend pas à gérer </t>
+  </si>
+  <si>
+    <t>Orienté web</t>
+  </si>
+  <si>
+    <t>La gateway est paramétrée via une interface web donc administrable depuis n'importe quelle machine</t>
+  </si>
+  <si>
+    <t>Avis des utilisateurs</t>
+  </si>
+  <si>
+    <t>L'utilisateur choisit les appareils sur lesquels il veut activer le contrôle parental. Celui-ci consiste dans cette version standard à limiter les heures de navigation sur internet individuellement. Un créneau horaire peut être défini selon les jours de la semaine et du weekend ainsi que le temps total. Ce contrôle est paramétrable sur la swisscom TV box. Les émissions contenant des limites d'âge peuvent également être bloquées par un PIN que seules les personnes autorisées connaissent.</t>
+  </si>
+  <si>
+    <t>Bloque la navigation sur internet et certains contenus</t>
+  </si>
+  <si>
+    <t>Navigation internet -&gt; Pas directement. Si l'enfant utilise toujours les mêmes appareils, alors le contrôle est indirectement associé à l'âge.
+Blocage de contenu lié à l'âge -&gt; Oui</t>
+  </si>
+  <si>
+    <t>Aucun avis disponible</t>
+  </si>
+  <si>
+    <t>Payant</t>
+  </si>
+  <si>
+    <t>La fonctionnalité est comprise dans l'abonnement swisscom</t>
+  </si>
+  <si>
+    <t>Offline</t>
+  </si>
+  <si>
+    <t>Est inutile en hors ligne puisqu’il monitore
+uniquement ce qui est en ligne</t>
+  </si>
+  <si>
+    <t>Ce contrôle parental est facile d'utilisation. Par contre, il ne permet pas de filtrer spécifiquement le contenu (mis à part le blocage du contenu limité par l'âge). Internet security permet un contrôle beaucoup plus approfondi, c'est le prochain service analysé.</t>
+  </si>
+  <si>
+    <t>Internet Security Swisscom</t>
+  </si>
+  <si>
+    <t>Bonne application (4.4/5 sur google play)</t>
+  </si>
+  <si>
+    <t>Bloque l'accès à l'ordinateur, les heures de navigation sur internet et certains contenus</t>
+  </si>
+  <si>
+    <t>Application native</t>
+  </si>
+  <si>
+    <t>Fonctionne sur ordinateur, tablette et smartphone (fonctionnalités différentes)</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne donne aucun contrôle. Le service
+interdit mais n'apprend pas à gérer </t>
+  </si>
+  <si>
+    <t>Facile à utiliser</t>
+  </si>
+  <si>
+    <t>La fonctionnalité est gratuite pendant 6 mois et ensuite payante</t>
+  </si>
+  <si>
+    <t>Utile car restreint également l'accès à la machine et pas seulement internet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette application est également très utile pour la protection des données et contre les sites webs dangereux ainsi que les virus. </t>
+  </si>
+  <si>
+    <t>L'utilisateur installe cette application sur la machine que l'enfant ou l'adolescent utilise depuis le compte administrateur. L'application définit le contenu non-accessible par catégories et par sites spécifiques. Elle permet aussi de définir les horaires de navigation sur internet et d'accès à la machine même.</t>
   </si>
 </sst>
 </file>
@@ -426,14 +515,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -446,27 +535,58 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -735,46 +855,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="2:4" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="2:4" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -790,7 +910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -798,7 +918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,7 +926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="56" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -814,7 +934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -822,7 +942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
@@ -833,7 +953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
@@ -841,7 +961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -849,7 +969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -857,49 +977,49 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="13"/>
     </row>
-    <row r="21" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="2:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="70" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,7 +1027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
@@ -915,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
@@ -923,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" ht="51" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
@@ -931,7 +1051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" ht="51" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
@@ -939,7 +1059,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
@@ -947,7 +1067,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
@@ -955,7 +1075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -963,7 +1083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
@@ -971,7 +1091,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
@@ -979,20 +1099,319 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="2:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+    <row r="35" spans="2:3" ht="66.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="39" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="15"/>
+    </row>
+    <row r="42" spans="2:3" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="11"/>
+    </row>
+    <row r="58" spans="2:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="60" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="13"/>
+    </row>
+    <row r="62" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="15"/>
+    </row>
+    <row r="63" spans="2:3" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="17"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" s="11"/>
+    </row>
+    <row r="79" spans="2:3" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="20">
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -1000,12 +1419,9 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>